<commit_message>
Final Update Project Report
</commit_message>
<xml_diff>
--- a/Documents/Presence Questionnaires/Presence Questionnaire-1.xlsx
+++ b/Documents/Presence Questionnaires/Presence Questionnaire-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/RVA/Projeto/VRTK-Furniture-Assembly/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/RVA/Projeto/VRTK-Furniture-Assembly/Documents/Presence Questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010ADD1E-EBE1-1640-B72D-FA34B3485C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9270551-2679-2D47-8AE1-A436CAC77ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{912E7241-D3F4-AB46-825B-DD7B8B756328}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{912E7241-D3F4-AB46-825B-DD7B8B756328}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1152FE-8D98-0643-B41D-CEC7F8533EC0}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>